<commit_message>
jogos, batedores e noticias
</commit_message>
<xml_diff>
--- a/Lista Batedores.xlsx
+++ b/Lista Batedores.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\OneDrive\Área de Trabalho\Cursos TI\Site_FPL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Times</t>
   </si>
@@ -120,9 +125,6 @@
     <t>Milner - Salah</t>
   </si>
   <si>
-    <t>CR7 - Bruno Fernandes</t>
-  </si>
-  <si>
     <t>Wilson - Wood</t>
   </si>
   <si>
@@ -253,6 +255,12 @@
   </si>
   <si>
     <t>Haaland - KDB - Mahrez</t>
+  </si>
+  <si>
+    <t>Bruno Fernandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bruno Fernandes</t>
   </si>
 </sst>
 </file>
@@ -530,6 +538,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -577,7 +588,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,7 +623,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -823,20 +834,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -847,10 +858,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -858,13 +869,13 @@
         <v>23</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -872,13 +883,13 @@
         <v>24</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -886,13 +897,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -900,27 +911,27 @@
         <v>26</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -928,13 +939,13 @@
         <v>27</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -942,13 +953,13 @@
         <v>28</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -956,13 +967,13 @@
         <v>29</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -970,13 +981,13 @@
         <v>30</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
@@ -984,13 +995,13 @@
         <v>31</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
@@ -998,13 +1009,13 @@
         <v>32</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1012,125 +1023,125 @@
         <v>33</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="23" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1143,7 +1154,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1155,7 +1166,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>